<commit_message>
new tours demo test data sheet updated
</commit_message>
<xml_diff>
--- a/NewTours_Demo/src/test/java/com/pack/Datasheet/TestData.xlsx
+++ b/NewTours_Demo/src/test/java/com/pack/Datasheet/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
   <si>
     <t>sl_no</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Unified Airlines</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1668,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
@@ -2136,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2264,7 +2267,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -2356,7 +2359,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>

</xml_diff>